<commit_message>
Added Kerr 6th floor machine numbers and stuff
Made it loop through the excel file row by row and create a list of all machines with our unique name scheme. Should work w python 3
</commit_message>
<xml_diff>
--- a/src/exampleSheet.xlsx
+++ b/src/exampleSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jduval/Documents/GitHub/laundrylocator/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F4677D7-27FD-EF4B-8E2B-FCDE65B69372}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635EA055-A49B-814D-8430-37CEF156D04B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{2529F8DE-B5D4-C349-BC7C-7C59B69925B0}"/>
+    <workbookView xWindow="2760" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{2529F8DE-B5D4-C349-BC7C-7C59B69925B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Building Name</t>
   </si>
@@ -48,7 +48,16 @@
     <t>A</t>
   </si>
   <si>
-    <t>xxx-xxx</t>
+    <t>213-GKD</t>
+  </si>
+  <si>
+    <t>214-GKD</t>
+  </si>
+  <si>
+    <t>215-GKD</t>
+  </si>
+  <si>
+    <t>216-GKD</t>
   </si>
 </sst>
 </file>
@@ -400,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828515AF-E36C-0D44-BEAD-1C1FF3A257F2}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,6 +451,57 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Put some Kerr info on spreadsheet
</commit_message>
<xml_diff>
--- a/src/exampleSheet.xlsx
+++ b/src/exampleSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jduval/Documents/GitHub/laundrylocator/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635EA055-A49B-814D-8430-37CEF156D04B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AB3D80-BE5F-9E43-B3B4-5AE6B2BC8204}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2760" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{2529F8DE-B5D4-C349-BC7C-7C59B69925B0}"/>
   </bookViews>
@@ -412,7 +412,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>